<commit_message>
VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_SubjectIsAPotentialRoundTrip - Final - 3rd June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9427BD6B-3149-49F1-B43F-F7E1D32F64F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D187CA67-CD07-4F50-9D41-1198DDF5318D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="104">
   <si>
     <t>Subject</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round-trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to Capital Provider because it is being considered to be a potential Roundtrip</t>
+  </si>
+  <si>
+    <t>Comment2</t>
   </si>
 </sst>
 </file>
@@ -844,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1509,32 +1515,39 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>89</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mid - 3rd June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D187CA67-CD07-4F50-9D41-1198DDF5318D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED3CAE1-DD53-40DD-8822-09D6811AA3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="105">
   <si>
     <t>Subject</t>
   </si>
@@ -343,19 +343,22 @@
     <t>Warning Msg 2</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round-trip candidate, no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
     <t>Warning Msg 3</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round-trip candidate no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
-    <t>Requesting to change Company Type to Capital Provider because it is being considered to be a potential Roundtrip</t>
-  </si>
-  <si>
     <t>Comment2</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm.</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +871,7 @@
         <v>98</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -876,10 +879,10 @@
         <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1515,20 +1518,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="3" max="4" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>87</v>
       </c>
@@ -1536,10 +1539,13 @@
         <v>88</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>90</v>
       </c>
@@ -1548,6 +1554,9 @@
       </c>
       <c r="C2" s="9" t="s">
         <v>102</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>